<commit_message>
Read from PDF with PDF Activity
</commit_message>
<xml_diff>
--- a/lib/net45/Data/Config.xlsx
+++ b/lib/net45/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grouperenault-my.sharepoint.com/personal/george-cristian_ceapa_dacia_com/Documents/3. RPA/2. Proiecte in dezvoltare/5. MQD/Program/Exemple/DRPCIV_Export_modif/lib/net45/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grouperenault-my.sharepoint.com/personal/george-cristian_ceapa_dacia_com/Documents/3. RPA/2. Proiecte in dezvoltare/5. MQD/Program/Exemple/MQD/lib/net45/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{62C6AB15-444F-490E-A99F-EE489BC53427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB926027-B10D-499F-AD17-AAFF2EAAE709}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{62C6AB15-444F-490E-A99F-EE489BC53427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1F61E82-49AE-4EB9-A1B6-FAC9C4056B58}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2064" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -207,9 +207,6 @@
     <t>Process Name for mail</t>
   </si>
   <si>
-    <t>_Autoturisme;_Autobuze_Microbuze;_Autovehicule_Marfuri;_Vehicule_Speciale</t>
-  </si>
-  <si>
     <t>filesNames</t>
   </si>
   <si>
@@ -261,9 +258,6 @@
     <t>george-cristian.ceapa@dacia.com</t>
   </si>
   <si>
-    <t>\\lab3D01\lab3d\CV_TL\Wenzel_3_232837V_G11244\PDFResults</t>
-  </si>
-  <si>
     <t>D:\Public\MQD\Server\</t>
   </si>
   <si>
@@ -274,6 +268,21 @@
   </si>
   <si>
     <t>\Alliance\BARC Romania Network - 00. RobotWork\MQD\Results</t>
+  </si>
+  <si>
+    <t>exportLocation</t>
+  </si>
+  <si>
+    <t>D:\Public\MQD\Import\</t>
+  </si>
+  <si>
+    <t>SharePointLocalPath</t>
+  </si>
+  <si>
+    <t>\lab3D01\lab3d\CV_TL\Wenzel_3_232837V_G11244\PDFResults</t>
+  </si>
+  <si>
+    <t>Arbre; Arbore</t>
   </si>
 </sst>
 </file>
@@ -672,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z32"/>
+  <dimension ref="A1:Z35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -739,10 +748,10 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>59</v>
@@ -753,7 +762,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>22</v>
@@ -792,124 +801,135 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
-      <c r="A14" s="6" t="s">
+    <row r="15" spans="1:26">
+      <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26">
-      <c r="A16" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="6" t="s">
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C21" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="9" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="C31" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="8" t="s">
+      <c r="C35" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1" xr:uid="{64300853-7A18-4755-B1D0-05F4E95E669D}"/>
-    <hyperlink ref="B26" r:id="rId2" xr:uid="{B710F653-C8CB-4ED5-AD86-7B14997867E9}"/>
+    <hyperlink ref="B21" r:id="rId1" xr:uid="{64300853-7A18-4755-B1D0-05F4E95E669D}"/>
+    <hyperlink ref="B29" r:id="rId2" display="\\lab3D01\lab3d\CV_TL\Wenzel_3_232837V_G11244\PDFResults" xr:uid="{B710F653-C8CB-4ED5-AD86-7B14997867E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>